<commit_message>
Changed screen shots to same month
</commit_message>
<xml_diff>
--- a/darkSkyTimes.xlsx
+++ b/darkSkyTimes.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:F33"/>
+  <dimension ref="A2:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -480,22 +480,22 @@
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>2023/04/01 05:33</t>
+          <t>2023/05/01 04:46</t>
         </is>
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>2023/04/01 21:27</t>
+          <t>2023/05/01 22:10</t>
         </is>
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>2023/04/01 05:38</t>
+          <t>2023/05/01 04:41</t>
         </is>
       </c>
       <c r="E3" s="2" t="inlineStr">
         <is>
-          <t>2023/04/01 15:31</t>
+          <t>2023/05/01 16:25</t>
         </is>
       </c>
     </row>
@@ -505,22 +505,22 @@
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>2023/04/02 05:59</t>
+          <t>2023/05/02 05:06</t>
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>2023/04/02 21:28</t>
+          <t>2023/05/02 22:11</t>
         </is>
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>2023/04/02 05:36</t>
+          <t>2023/05/02 04:40</t>
         </is>
       </c>
       <c r="E4" s="2" t="inlineStr">
         <is>
-          <t>2023/04/02 16:34</t>
+          <t>2023/05/02 17:28</t>
         </is>
       </c>
     </row>
@@ -530,22 +530,22 @@
       </c>
       <c r="B5" s="2" t="inlineStr">
         <is>
-          <t>2023/04/03 06:21</t>
+          <t>2023/05/03 05:27</t>
         </is>
       </c>
       <c r="C5" s="2" t="inlineStr">
         <is>
-          <t>2023/04/03 21:29</t>
+          <t>2023/05/03 22:13</t>
         </is>
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>2023/04/03 05:34</t>
+          <t>2023/05/03 04:38</t>
         </is>
       </c>
       <c r="E5" s="2" t="inlineStr">
         <is>
-          <t>2023/04/03 17:36</t>
+          <t>2023/05/03 18:33</t>
         </is>
       </c>
     </row>
@@ -555,22 +555,22 @@
       </c>
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>2023/04/04 06:42</t>
+          <t>2023/05/04 05:49</t>
         </is>
       </c>
       <c r="C6" s="2" t="inlineStr">
         <is>
-          <t>2023/04/04 21:31</t>
+          <t>2023/05/04 22:14</t>
         </is>
       </c>
       <c r="D6" s="2" t="inlineStr">
         <is>
-          <t>2023/04/04 05:32</t>
+          <t>2023/05/04 04:36</t>
         </is>
       </c>
       <c r="E6" s="2" t="inlineStr">
         <is>
-          <t>2023/04/04 18:39</t>
+          <t>2023/05/04 19:41</t>
         </is>
       </c>
     </row>
@@ -580,22 +580,22 @@
       </c>
       <c r="B7" s="2" t="inlineStr">
         <is>
-          <t>2023/04/05 07:03</t>
+          <t>2023/05/05 06:15</t>
         </is>
       </c>
       <c r="C7" s="2" t="inlineStr">
         <is>
-          <t>2023/04/05 21:32</t>
+          <t>2023/05/05 22:16</t>
         </is>
       </c>
       <c r="D7" s="2" t="inlineStr">
         <is>
-          <t>2023/04/05 05:30</t>
+          <t>2023/05/05 04:34</t>
         </is>
       </c>
       <c r="E7" s="2" t="inlineStr">
         <is>
-          <t>2023/04/05 19:43</t>
+          <t>2023/05/05 20:53</t>
         </is>
       </c>
     </row>
@@ -605,22 +605,22 @@
       </c>
       <c r="B8" s="2" t="inlineStr">
         <is>
-          <t>2023/04/06 07:24</t>
+          <t>2023/05/06 06:45</t>
         </is>
       </c>
       <c r="C8" s="2" t="inlineStr">
         <is>
-          <t>2023/04/06 21:33</t>
+          <t>2023/05/06 22:18</t>
         </is>
       </c>
       <c r="D8" s="2" t="inlineStr">
         <is>
-          <t>2023/04/06 05:28</t>
+          <t>2023/05/06 04:33</t>
         </is>
       </c>
       <c r="E8" s="2" t="inlineStr">
         <is>
-          <t>2023/04/06 20:49</t>
+          <t>2023/05/06 22:07</t>
         </is>
       </c>
     </row>
@@ -630,22 +630,22 @@
       </c>
       <c r="B9" s="2" t="inlineStr">
         <is>
-          <t>2023/04/07 07:47</t>
+          <t>2023/05/07 07:23</t>
         </is>
       </c>
       <c r="C9" s="2" t="inlineStr">
         <is>
-          <t>2023/04/07 21:35</t>
+          <t>2023/05/07 22:19</t>
         </is>
       </c>
       <c r="D9" s="2" t="inlineStr">
         <is>
-          <t>2023/04/07 05:26</t>
+          <t>2023/05/07 04:31</t>
         </is>
       </c>
       <c r="E9" s="2" t="inlineStr">
         <is>
-          <t>2023/04/07 21:57</t>
+          <t>2023/05/07 23:20</t>
         </is>
       </c>
     </row>
@@ -655,22 +655,17 @@
       </c>
       <c r="B10" s="2" t="inlineStr">
         <is>
-          <t>2023/04/08 08:13</t>
+          <t>2023/05/08 08:12</t>
         </is>
       </c>
       <c r="C10" s="2" t="inlineStr">
         <is>
-          <t>2023/04/08 21:36</t>
+          <t>2023/05/08 22:21</t>
         </is>
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>2023/04/08 05:24</t>
-        </is>
-      </c>
-      <c r="E10" s="2" t="inlineStr">
-        <is>
-          <t>2023/04/08 23:08</t>
+          <t>2023/05/08 04:29</t>
         </is>
       </c>
     </row>
@@ -680,17 +675,22 @@
       </c>
       <c r="B11" s="2" t="inlineStr">
         <is>
-          <t>2023/04/09 08:46</t>
+          <t>2023/05/09 09:12</t>
         </is>
       </c>
       <c r="C11" s="2" t="inlineStr">
         <is>
-          <t>2023/04/09 21:37</t>
+          <t>2023/05/09 22:22</t>
         </is>
       </c>
       <c r="D11" s="2" t="inlineStr">
         <is>
-          <t>2023/04/09 05:23</t>
+          <t>2023/05/09 04:28</t>
+        </is>
+      </c>
+      <c r="E11" s="2" t="inlineStr">
+        <is>
+          <t>2023/05/09 00:29</t>
         </is>
       </c>
     </row>
@@ -700,22 +700,22 @@
       </c>
       <c r="B12" s="2" t="inlineStr">
         <is>
-          <t>2023/04/10 09:26</t>
+          <t>2023/05/10 10:22</t>
         </is>
       </c>
       <c r="C12" s="2" t="inlineStr">
         <is>
-          <t>2023/04/10 21:39</t>
+          <t>2023/05/10 22:24</t>
         </is>
       </c>
       <c r="D12" s="2" t="inlineStr">
         <is>
-          <t>2023/04/10 05:21</t>
+          <t>2023/05/10 04:26</t>
         </is>
       </c>
       <c r="E12" s="2" t="inlineStr">
         <is>
-          <t>2023/04/10 00:21</t>
+          <t>2023/05/10 01:27</t>
         </is>
       </c>
     </row>
@@ -725,22 +725,22 @@
       </c>
       <c r="B13" s="2" t="inlineStr">
         <is>
-          <t>2023/04/11 10:18</t>
+          <t>2023/05/11 11:37</t>
         </is>
       </c>
       <c r="C13" s="2" t="inlineStr">
         <is>
-          <t>2023/04/11 21:40</t>
+          <t>2023/05/11 22:25</t>
         </is>
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>2023/04/11 05:19</t>
+          <t>2023/05/11 04:24</t>
         </is>
       </c>
       <c r="E13" s="2" t="inlineStr">
         <is>
-          <t>2023/04/11 01:31</t>
+          <t>2023/05/11 02:15</t>
         </is>
       </c>
     </row>
@@ -750,22 +750,22 @@
       </c>
       <c r="B14" s="2" t="inlineStr">
         <is>
-          <t>2023/04/12 11:20</t>
+          <t>2023/05/12 12:54</t>
         </is>
       </c>
       <c r="C14" s="2" t="inlineStr">
         <is>
-          <t>2023/04/12 21:42</t>
+          <t>2023/05/12 22:27</t>
         </is>
       </c>
       <c r="D14" s="2" t="inlineStr">
         <is>
-          <t>2023/04/12 05:17</t>
+          <t>2023/05/12 04:23</t>
         </is>
       </c>
       <c r="E14" s="2" t="inlineStr">
         <is>
-          <t>2023/04/12 02:36</t>
+          <t>2023/05/12 02:53</t>
         </is>
       </c>
     </row>
@@ -775,22 +775,22 @@
       </c>
       <c r="B15" s="2" t="inlineStr">
         <is>
-          <t>2023/04/13 12:31</t>
+          <t>2023/05/13 14:09</t>
         </is>
       </c>
       <c r="C15" s="2" t="inlineStr">
         <is>
-          <t>2023/04/13 21:43</t>
+          <t>2023/05/13 22:28</t>
         </is>
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>2023/04/13 05:15</t>
+          <t>2023/05/13 04:21</t>
         </is>
       </c>
       <c r="E15" s="2" t="inlineStr">
         <is>
-          <t>2023/04/13 03:30</t>
+          <t>2023/05/13 03:23</t>
         </is>
       </c>
     </row>
@@ -800,22 +800,22 @@
       </c>
       <c r="B16" s="2" t="inlineStr">
         <is>
-          <t>2023/04/14 13:48</t>
+          <t>2023/05/14 15:22</t>
         </is>
       </c>
       <c r="C16" s="2" t="inlineStr">
         <is>
-          <t>2023/04/14 21:44</t>
+          <t>2023/05/14 22:30</t>
         </is>
       </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
-          <t>2023/04/14 05:13</t>
+          <t>2023/05/14 04:20</t>
         </is>
       </c>
       <c r="E16" s="2" t="inlineStr">
         <is>
-          <t>2023/04/14 04:14</t>
+          <t>2023/05/14 03:50</t>
         </is>
       </c>
     </row>
@@ -825,22 +825,22 @@
       </c>
       <c r="B17" s="2" t="inlineStr">
         <is>
-          <t>2023/04/15 15:05</t>
+          <t>2023/05/15 16:33</t>
         </is>
       </c>
       <c r="C17" s="2" t="inlineStr">
         <is>
-          <t>2023/04/15 21:46</t>
+          <t>2023/05/15 22:32</t>
         </is>
       </c>
       <c r="D17" s="2" t="inlineStr">
         <is>
-          <t>2023/04/15 05:11</t>
+          <t>2023/05/15 04:18</t>
         </is>
       </c>
       <c r="E17" s="2" t="inlineStr">
         <is>
-          <t>2023/04/15 04:50</t>
+          <t>2023/05/15 04:13</t>
         </is>
       </c>
     </row>
@@ -850,22 +850,22 @@
       </c>
       <c r="B18" s="2" t="inlineStr">
         <is>
-          <t>2023/04/16 16:21</t>
+          <t>2023/05/16 17:43</t>
         </is>
       </c>
       <c r="C18" s="2" t="inlineStr">
         <is>
-          <t>2023/04/16 21:47</t>
+          <t>2023/05/16 22:33</t>
         </is>
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>2023/04/16 05:09</t>
+          <t>2023/05/16 04:17</t>
         </is>
       </c>
       <c r="E18" s="2" t="inlineStr">
         <is>
-          <t>2023/04/16 05:20</t>
+          <t>2023/05/16 04:36</t>
         </is>
       </c>
     </row>
@@ -875,22 +875,22 @@
       </c>
       <c r="B19" s="2" t="inlineStr">
         <is>
-          <t>2023/04/17 17:35</t>
+          <t>2023/05/17 18:54</t>
         </is>
       </c>
       <c r="C19" s="2" t="inlineStr">
         <is>
-          <t>2023/04/17 21:49</t>
+          <t>2023/05/17 22:35</t>
         </is>
       </c>
       <c r="D19" s="2" t="inlineStr">
         <is>
-          <t>2023/04/17 05:07</t>
+          <t>2023/05/17 04:15</t>
         </is>
       </c>
       <c r="E19" s="2" t="inlineStr">
         <is>
-          <t>2023/04/17 05:46</t>
+          <t>2023/05/17 05:00</t>
         </is>
       </c>
     </row>
@@ -900,22 +900,22 @@
       </c>
       <c r="B20" s="2" t="inlineStr">
         <is>
-          <t>2023/04/18 18:47</t>
+          <t>2023/05/18 20:05</t>
         </is>
       </c>
       <c r="C20" s="2" t="inlineStr">
         <is>
-          <t>2023/04/18 21:50</t>
+          <t>2023/05/18 22:36</t>
         </is>
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>2023/04/18 05:05</t>
+          <t>2023/05/18 04:14</t>
         </is>
       </c>
       <c r="E20" s="2" t="inlineStr">
         <is>
-          <t>2023/04/18 06:10</t>
+          <t>2023/05/18 05:26</t>
         </is>
       </c>
     </row>
@@ -925,22 +925,22 @@
       </c>
       <c r="B21" s="2" t="inlineStr">
         <is>
-          <t>2023/04/19 19:59</t>
+          <t>2023/05/19 21:14</t>
         </is>
       </c>
       <c r="C21" s="2" t="inlineStr">
         <is>
-          <t>2023/04/19 21:52</t>
+          <t>2023/05/19 22:38</t>
         </is>
       </c>
       <c r="D21" s="2" t="inlineStr">
         <is>
-          <t>2023/04/19 05:04</t>
+          <t>2023/05/19 04:12</t>
         </is>
       </c>
       <c r="E21" s="2" t="inlineStr">
         <is>
-          <t>2023/04/19 06:33</t>
+          <t>2023/05/19 05:56</t>
         </is>
       </c>
     </row>
@@ -950,22 +950,22 @@
       </c>
       <c r="B22" s="2" t="inlineStr">
         <is>
-          <t>2023/04/20 21:12</t>
+          <t>2023/05/20 22:21</t>
         </is>
       </c>
       <c r="C22" s="2" t="inlineStr">
         <is>
-          <t>2023/04/20 21:53</t>
+          <t>2023/05/20 22:39</t>
         </is>
       </c>
       <c r="D22" s="2" t="inlineStr">
         <is>
-          <t>2023/04/20 05:02</t>
+          <t>2023/05/20 04:11</t>
         </is>
       </c>
       <c r="E22" s="2" t="inlineStr">
         <is>
-          <t>2023/04/20 06:58</t>
+          <t>2023/05/20 06:32</t>
         </is>
       </c>
     </row>
@@ -975,22 +975,22 @@
       </c>
       <c r="B23" s="2" t="inlineStr">
         <is>
-          <t>2023/04/21 22:23</t>
+          <t>2023/05/21 23:22</t>
         </is>
       </c>
       <c r="C23" s="2" t="inlineStr">
         <is>
-          <t>2023/04/21 21:55</t>
+          <t>2023/05/21 22:41</t>
         </is>
       </c>
       <c r="D23" s="2" t="inlineStr">
         <is>
-          <t>2023/04/21 05:00</t>
+          <t>2023/05/21 04:10</t>
         </is>
       </c>
       <c r="E23" s="2" t="inlineStr">
         <is>
-          <t>2023/04/21 07:26</t>
+          <t>2023/05/21 07:14</t>
         </is>
       </c>
     </row>
@@ -998,24 +998,19 @@
       <c r="A24" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="B24" s="2" t="inlineStr">
-        <is>
-          <t>2023/04/22 23:32</t>
-        </is>
-      </c>
       <c r="C24" s="2" t="inlineStr">
         <is>
-          <t>2023/04/22 21:56</t>
+          <t>2023/05/22 22:42</t>
         </is>
       </c>
       <c r="D24" s="2" t="inlineStr">
         <is>
-          <t>2023/04/22 04:58</t>
+          <t>2023/05/22 04:08</t>
         </is>
       </c>
       <c r="E24" s="2" t="inlineStr">
         <is>
-          <t>2023/04/22 07:59</t>
+          <t>2023/05/22 08:04</t>
         </is>
       </c>
     </row>
@@ -1023,19 +1018,24 @@
       <c r="A25" s="1" t="n">
         <v>23</v>
       </c>
+      <c r="B25" s="2" t="inlineStr">
+        <is>
+          <t>2023/05/23 00:14</t>
+        </is>
+      </c>
       <c r="C25" s="2" t="inlineStr">
         <is>
-          <t>2023/04/23 21:58</t>
+          <t>2023/05/23 22:43</t>
         </is>
       </c>
       <c r="D25" s="2" t="inlineStr">
         <is>
-          <t>2023/04/23 04:56</t>
+          <t>2023/05/23 04:07</t>
         </is>
       </c>
       <c r="E25" s="2" t="inlineStr">
         <is>
-          <t>2023/04/23 08:37</t>
+          <t>2023/05/23 09:01</t>
         </is>
       </c>
     </row>
@@ -1045,22 +1045,22 @@
       </c>
       <c r="B26" s="2" t="inlineStr">
         <is>
-          <t>2023/04/24 00:36</t>
+          <t>2023/05/24 00:58</t>
         </is>
       </c>
       <c r="C26" s="2" t="inlineStr">
         <is>
-          <t>2023/04/24 21:59</t>
+          <t>2023/05/24 22:45</t>
         </is>
       </c>
       <c r="D26" s="2" t="inlineStr">
         <is>
-          <t>2023/04/24 04:54</t>
+          <t>2023/05/24 04:06</t>
         </is>
       </c>
       <c r="E26" s="2" t="inlineStr">
         <is>
-          <t>2023/04/24 09:23</t>
+          <t>2023/05/24 10:02</t>
         </is>
       </c>
     </row>
@@ -1070,22 +1070,22 @@
       </c>
       <c r="B27" s="2" t="inlineStr">
         <is>
-          <t>2023/04/25 01:33</t>
+          <t>2023/05/25 01:33</t>
         </is>
       </c>
       <c r="C27" s="2" t="inlineStr">
         <is>
-          <t>2023/04/25 22:01</t>
+          <t>2023/05/25 22:46</t>
         </is>
       </c>
       <c r="D27" s="2" t="inlineStr">
         <is>
-          <t>2023/04/25 04:52</t>
+          <t>2023/05/25 04:05</t>
         </is>
       </c>
       <c r="E27" s="2" t="inlineStr">
         <is>
-          <t>2023/04/25 10:15</t>
+          <t>2023/05/25 11:04</t>
         </is>
       </c>
     </row>
@@ -1095,22 +1095,22 @@
       </c>
       <c r="B28" s="2" t="inlineStr">
         <is>
-          <t>2023/04/26 02:22</t>
+          <t>2023/05/26 02:02</t>
         </is>
       </c>
       <c r="C28" s="2" t="inlineStr">
         <is>
-          <t>2023/04/26 22:02</t>
+          <t>2023/05/26 22:48</t>
         </is>
       </c>
       <c r="D28" s="2" t="inlineStr">
         <is>
-          <t>2023/04/26 04:51</t>
+          <t>2023/05/26 04:03</t>
         </is>
       </c>
       <c r="E28" s="2" t="inlineStr">
         <is>
-          <t>2023/04/26 11:13</t>
+          <t>2023/05/26 12:07</t>
         </is>
       </c>
     </row>
@@ -1120,22 +1120,22 @@
       </c>
       <c r="B29" s="2" t="inlineStr">
         <is>
-          <t>2023/04/27 03:01</t>
+          <t>2023/05/27 02:27</t>
         </is>
       </c>
       <c r="C29" s="2" t="inlineStr">
         <is>
-          <t>2023/04/27 22:04</t>
+          <t>2023/05/27 22:49</t>
         </is>
       </c>
       <c r="D29" s="2" t="inlineStr">
         <is>
-          <t>2023/04/27 04:49</t>
+          <t>2023/05/27 04:02</t>
         </is>
       </c>
       <c r="E29" s="2" t="inlineStr">
         <is>
-          <t>2023/04/27 12:15</t>
+          <t>2023/05/27 13:09</t>
         </is>
       </c>
     </row>
@@ -1145,22 +1145,22 @@
       </c>
       <c r="B30" s="2" t="inlineStr">
         <is>
-          <t>2023/04/28 03:34</t>
+          <t>2023/05/28 02:49</t>
         </is>
       </c>
       <c r="C30" s="2" t="inlineStr">
         <is>
-          <t>2023/04/28 22:05</t>
+          <t>2023/05/28 22:50</t>
         </is>
       </c>
       <c r="D30" s="2" t="inlineStr">
         <is>
-          <t>2023/04/28 04:47</t>
+          <t>2023/05/28 04:01</t>
         </is>
       </c>
       <c r="E30" s="2" t="inlineStr">
         <is>
-          <t>2023/04/28 13:17</t>
+          <t>2023/05/28 14:10</t>
         </is>
       </c>
     </row>
@@ -1170,22 +1170,22 @@
       </c>
       <c r="B31" s="2" t="inlineStr">
         <is>
-          <t>2023/04/29 04:01</t>
+          <t>2023/05/29 03:09</t>
         </is>
       </c>
       <c r="C31" s="2" t="inlineStr">
         <is>
-          <t>2023/04/29 22:07</t>
+          <t>2023/05/29 22:52</t>
         </is>
       </c>
       <c r="D31" s="2" t="inlineStr">
         <is>
-          <t>2023/04/29 04:45</t>
+          <t>2023/05/29 04:00</t>
         </is>
       </c>
       <c r="E31" s="2" t="inlineStr">
         <is>
-          <t>2023/04/30 15:22</t>
+          <t>2023/05/29 15:12</t>
         </is>
       </c>
     </row>
@@ -1195,23 +1195,48 @@
       </c>
       <c r="B32" s="2" t="inlineStr">
         <is>
-          <t>2023/05/01 04:46</t>
+          <t>2023/05/30 03:29</t>
         </is>
       </c>
       <c r="C32" s="2" t="inlineStr">
         <is>
-          <t>2023/04/30 22:08</t>
+          <t>2023/05/30 22:53</t>
         </is>
       </c>
       <c r="D32" s="2" t="inlineStr">
         <is>
-          <t>2023/04/30 04:43</t>
+          <t>2023/05/30 03:59</t>
+        </is>
+      </c>
+      <c r="E32" s="2" t="inlineStr">
+        <is>
+          <t>2023/05/31 17:22</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
         <v>31</v>
+      </c>
+      <c r="B33" s="2" t="inlineStr">
+        <is>
+          <t>2023/06/01 04:14</t>
+        </is>
+      </c>
+      <c r="C33" s="2" t="inlineStr">
+        <is>
+          <t>2023/05/31 22:54</t>
+        </is>
+      </c>
+      <c r="D33" s="2" t="inlineStr">
+        <is>
+          <t>2023/05/31 03:58</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>